<commit_message>
download weekly on sundays
</commit_message>
<xml_diff>
--- a/BNP Excel Sheet.xlsx
+++ b/BNP Excel Sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="192">
   <si>
     <t>RunID</t>
   </si>
@@ -444,19 +444,22 @@
     <t>Turtlebeach</t>
   </si>
   <si>
+    <t>TURTLE BEACH</t>
+  </si>
+  <si>
+    <t>Turtle Beach</t>
+  </si>
+  <si>
+    <t>AccountID</t>
+  </si>
+  <si>
+    <t>HIH LOGISTICS, INC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International Textile &amp; Apparel </t>
+  </si>
+  <si>
     <t xml:space="preserve">TURTLE BEACH </t>
-  </si>
-  <si>
-    <t>Turtle Beach</t>
-  </si>
-  <si>
-    <t>AccountID</t>
-  </si>
-  <si>
-    <t>HIH LOGISTICS, INC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">International Textile &amp; Apparel </t>
   </si>
   <si>
     <t>FacilityID</t>
@@ -990,16 +993,16 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
@@ -1010,10 +1013,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
@@ -1024,10 +1027,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -1038,10 +1041,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -1052,10 +1055,10 @@
         <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
@@ -1066,10 +1069,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
@@ -1080,10 +1083,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
@@ -1094,10 +1097,10 @@
         <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
@@ -1108,10 +1111,10 @@
         <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
@@ -1122,10 +1125,10 @@
         <v>35</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
@@ -1136,10 +1139,10 @@
         <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
@@ -1150,10 +1153,10 @@
         <v>46</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
@@ -1164,10 +1167,10 @@
         <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
@@ -1178,10 +1181,10 @@
         <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
@@ -1192,10 +1195,10 @@
         <v>73</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
@@ -1206,10 +1209,10 @@
         <v>78</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
@@ -1220,10 +1223,10 @@
         <v>91</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
@@ -1234,10 +1237,10 @@
         <v>94</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
@@ -1248,10 +1251,10 @@
         <v>105</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
@@ -1262,10 +1265,10 @@
         <v>114</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
@@ -1276,10 +1279,10 @@
         <v>124</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
@@ -1290,10 +1293,10 @@
         <v>127</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1745,7 +1748,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>